<commit_message>
#3 #1 Created a roadmap for the rest of the year and added new classes to heatingsystem. Made notes about the meeting with Athanasios
</commit_message>
<xml_diff>
--- a/OntologyInput/DDINGS Greenhouse keywords.xlsx
+++ b/OntologyInput/DDINGS Greenhouse keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakkerrm\TNO\Data Driven INGS - Work\WP4 Datahub as uniform dataprovider\Greenhouse Ontology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakkerrm\git\ontology-dev\OntologyInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{56ED3591-60A8-4280-94D7-420A77B73D5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9C0111EB-BDE2-4BA2-A51D-D0C3BC7DBBF3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C168871-5F75-4DD2-9F36-C9555C6C5EA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{377206B5-75C8-478B-987E-9DAC5CB46A3C}"/>
   </bookViews>
@@ -30,17 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
   <si>
     <t>part of heating system</t>
   </si>
   <si>
-    <t>burner/boiler (equal or together)</t>
-  </si>
-  <si>
-    <t>provides the heat, similar to home boiler</t>
-  </si>
-  <si>
     <t>fuel</t>
   </si>
   <si>
@@ -110,25 +104,7 @@
     <t>measures the return temperature</t>
   </si>
   <si>
-    <t>boiler sensor</t>
-  </si>
-  <si>
-    <t>measures the temperature of the boiler</t>
-  </si>
-  <si>
-    <t>boiler supply sensor</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
     <t>connect heating system to the greenhouse</t>
-  </si>
-  <si>
-    <t>boiler circuit pump</t>
-  </si>
-  <si>
-    <t>part of boiler</t>
   </si>
   <si>
     <t>can be open or closed</t>
@@ -411,6 +387,132 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Climate Computer/ Control System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climate computer is dutch. Control system is better. The control system controls different functions and processes inside the greenhouse. For example for labout management. </t>
+  </si>
+  <si>
+    <t>Boiler supply sensor</t>
+  </si>
+  <si>
+    <t>boiler water temperature sensor</t>
+  </si>
+  <si>
+    <t>measures the temperature of the water inside the boiler. Sometimes if we don't use a manifold, then the boiler temperature is equal to the water supply temperature</t>
+  </si>
+  <si>
+    <t>measures the temperature of the water supplied by the boiler</t>
+  </si>
+  <si>
+    <t>heat water transport pump</t>
+  </si>
+  <si>
+    <t>Burner</t>
+  </si>
+  <si>
+    <t>Burns fuel to convert chemical energy to thermal energy.</t>
+  </si>
+  <si>
+    <t>boiler (equal or together)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provides the heat, similar to home boiler. Uses energy from the burner </t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For crop we should include family, gen, species, scientific name, </t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>Cogeneration Heat and Power</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cogeneration</t>
+  </si>
+  <si>
+    <t>Heat Exchanger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CirculationPump</t>
+  </si>
+  <si>
+    <t>part of boiler. Controlled with frequency controlled motor</t>
+  </si>
+  <si>
+    <t>Pump inside the Greenhouse to circulate the hot  water in the greenhouse. Operates with constant speed. In the climate computer this pump is on or off</t>
+  </si>
+  <si>
+    <t>Pump which is used to send the hot water fromt he main heating system to different greenhouse compartments upon request. More information in the climate computer that just on off</t>
+  </si>
+  <si>
+    <t>HeatingSystem</t>
+  </si>
+  <si>
+    <t>HeatingSystemPart</t>
+  </si>
+  <si>
+    <t>Substrate Heating</t>
+  </si>
+  <si>
+    <t>transport heating pipe</t>
+  </si>
+  <si>
+    <t>heating pipe that transports the heated water from the main heating system to the greenhouse compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary heating pipe </t>
+  </si>
+  <si>
+    <t>growing heating pipe</t>
+  </si>
+  <si>
+    <t>Heating pipe that is embedded in the floor of the greenhouse such that we warm up the floor. Usually concrete. Not very high temperature to not burn the roots, around 30</t>
+  </si>
+  <si>
+    <t>is used inside the greenhouse compartment to distribute the heated water.  Is around 60 degrees</t>
+  </si>
+  <si>
+    <t>is the heating pipe which has a diameter less than the primary heating pipe and is installed in the middle of the canopy and operates with relatively lower water temperatures around 40</t>
+  </si>
+  <si>
+    <t>embedded heating pipe/ floor heating</t>
+  </si>
+  <si>
+    <t>Greenhouse compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The area that is controlled in the same way regarding the climate. Can be separated with walls/screens or not. </t>
+  </si>
+  <si>
+    <t>Greenhouse zone/ irrigation zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone is inside a compartment, so the climate is controlled in the same way but the irrigation. Is the area inside a greenhouse compartment, can be part of all, where the same irrigation and fertigation strategy is applied. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenhouse block </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The group of area's where we apply the same control strategy. In a block we control certain variables in the same way. It has no direct relation to compartment and zone. </t>
+  </si>
+  <si>
+    <t>Greenhouse bench</t>
+  </si>
+  <si>
+    <t>The container in which the plant(s) is placed</t>
+  </si>
+  <si>
+    <t>GrowingSystemPart</t>
   </si>
 </sst>
 </file>
@@ -805,15 +907,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A844146E-EC52-4D55-856E-1184045B7F13}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="72.21875" customWidth="1"/>
     <col min="4" max="4" width="52.5546875" customWidth="1"/>
@@ -823,540 +925,549 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8">
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>29</v>
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G24" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="F26" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8">
       <c r="B27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G29" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="F33" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G33" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1"/>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G35" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="100.8">
       <c r="B36" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G36" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="86.4">
       <c r="B37" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G37" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1364,60 +1475,60 @@
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F40" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F41" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="43.2">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G46" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1425,76 +1536,76 @@
     </row>
     <row r="48" spans="1:7" ht="100.8">
       <c r="A48" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G48" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="129.6">
       <c r="A49" s="4"/>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G49" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="72">
       <c r="B50" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="129.6">
       <c r="B51" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G51" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="51">
       <c r="B52" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G52" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1502,72 +1613,193 @@
     </row>
     <row r="54" spans="1:7" ht="57.6">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G54" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="100.8">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="103.2">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F56" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="100.8">
       <c r="B57" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F57" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="42">
       <c r="B58" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F58" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="F63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1588,6 +1820,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Team Document" ma:contentTypeID="0x010100A35317DCC28344A7B82488658A034A5C010069E498006C15F040AAF23C596505DB08" ma:contentTypeVersion="15" ma:contentTypeDescription=" " ma:contentTypeScope="" ma:versionID="daae089886e5dfcdf91620598e62335c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b267fd-bbe0-4fe3-86fd-466470c14b02" xmlns:ns3="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7" xmlns:ns5="46c07ff3-5521-42af-a653-3855c83cb6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c787740b624ceaa53a6f81b9ff22a49" ns2:_="" ns3:_="" ns5:_="">
     <xsd:import namespace="64b267fd-bbe0-4fe3-86fd-466470c14b02"/>
@@ -1900,66 +2182,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TNOC_ClusterId xmlns="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7">060.28387</TNOC_ClusterId>
@@ -2002,7 +2225,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC4FB55-D490-49ED-AEAA-963B2A830DFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC7E6127-10A1-40C5-9CAC-A18D42DD8A37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2022,23 +2262,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC4FB55-D490-49ED-AEAA-963B2A830DFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C697E9F-13EF-41CB-B4FF-229AEE100FCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4CA6ED-F389-43A6-8E29-AA59BC0B8044}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2054,4 +2278,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C697E9F-13EF-41CB-B4FF-229AEE100FCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#2 Created a roadmap for the versions of the ontology until the end of the year
</commit_message>
<xml_diff>
--- a/OntologyInput/DDINGS Greenhouse keywords.xlsx
+++ b/OntologyInput/DDINGS Greenhouse keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakkerrm\git\ontology-dev\OntologyInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C168871-5F75-4DD2-9F36-C9555C6C5EA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D14089-735D-4801-A357-325F1B9C6372}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{377206B5-75C8-478B-987E-9DAC5CB46A3C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
   <si>
     <t>part of heating system</t>
   </si>
@@ -497,9 +497,6 @@
     <t>Greenhouse zone/ irrigation zone</t>
   </si>
   <si>
-    <t xml:space="preserve">Zone is inside a compartment, so the climate is controlled in the same way but the irrigation. Is the area inside a greenhouse compartment, can be part of all, where the same irrigation and fertigation strategy is applied. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Greenhouse block </t>
   </si>
   <si>
@@ -513,6 +510,33 @@
   </si>
   <si>
     <t>GrowingSystemPart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone is inside a compartment, so the climate is controlled in the same way but the irrigation. Is the area inside a greenhouse compartment, can be part of all, where the same irrigation and fertigation strategy is applied. Is not geographically decided </t>
+  </si>
+  <si>
+    <t>Heating source</t>
+  </si>
+  <si>
+    <t>geothermal energy</t>
+  </si>
+  <si>
+    <t>Hybrid systems</t>
+  </si>
+  <si>
+    <t>combines different energy sources for heat. E.g geothermal energy + fuel, or solar collectors</t>
+  </si>
+  <si>
+    <t>Heat pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid system that can be used for cooling and heating </t>
+  </si>
+  <si>
+    <t>passive system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system where you store energy without any device. Example thick wall to store warmth </t>
   </si>
 </sst>
 </file>
@@ -907,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A844146E-EC52-4D55-856E-1184045B7F13}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1780,26 +1804,58 @@
         <v>153</v>
       </c>
       <c r="C73" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="B74" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" t="s">
         <v>155</v>
-      </c>
-      <c r="C74" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" t="s">
         <v>157</v>
       </c>
-      <c r="C75" t="s">
-        <v>158</v>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Added all the keywords from the excel file
</commit_message>
<xml_diff>
--- a/OntologyInput/DDINGS Greenhouse keywords.xlsx
+++ b/OntologyInput/DDINGS Greenhouse keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakkerrm\git\ontology-dev\OntologyInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D14089-735D-4801-A357-325F1B9C6372}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A9895A-DB29-43C8-B044-FF5BAE4226E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{377206B5-75C8-478B-987E-9DAC5CB46A3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{377206B5-75C8-478B-987E-9DAC5CB46A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="171">
   <si>
     <t>part of heating system</t>
   </si>
@@ -537,6 +537,15 @@
   </si>
   <si>
     <t xml:space="preserve">system where you store energy without any device. Example thick wall to store warmth </t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Same for capacity: Where should this be? I think it's the property of a heating system</t>
+  </si>
+  <si>
+    <t>Do we need this in the ontology?</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -615,6 +622,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -931,944 +941,1005 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A844146E-EC52-4D55-856E-1184045B7F13}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="72.21875" customWidth="1"/>
-    <col min="4" max="4" width="52.5546875" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="39" style="2" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="56.25">
+      <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="H1" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="F3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="F4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="F5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="F6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="F7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="F8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="165">
+      <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8">
-      <c r="A10" t="s">
+      <c r="F9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
+      <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" t="s">
+      <c r="F11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8">
-      <c r="B13" t="s">
+      <c r="F12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" t="s">
+      <c r="F13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="F14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
+      <c r="F16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45">
+      <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" t="s">
+      <c r="F18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="F19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45">
+      <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" t="s">
+      <c r="F20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="B22" t="s">
+      <c r="F21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="90">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="28.8">
-      <c r="A23" t="s">
+      <c r="H22" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30">
+      <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="F23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F25" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="F26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28.8">
-      <c r="B27" t="s">
+      <c r="F25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="F26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30">
+      <c r="B27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="B28" t="s">
+      <c r="F27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="B29" t="s">
+      <c r="F28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="B30" t="s">
+      <c r="F29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30">
+      <c r="B30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="G30" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="F31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="120">
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="105">
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G33" t="s">
-        <v>116</v>
-      </c>
+      <c r="G33" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="F35" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="100.8">
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="B35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="B36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="B37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60">
+      <c r="A42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="86.4">
-      <c r="B37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="B40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="B41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="43.2">
-      <c r="A46" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:7" ht="100.8">
-      <c r="A48" s="4" t="s">
+      <c r="G42" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="120">
+      <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="C44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="135">
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="90">
+      <c r="B46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="165">
+      <c r="B47" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="56.25">
+      <c r="B48" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="C48" s="4" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="129.6">
-      <c r="A49" s="4"/>
-      <c r="B49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="72">
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>90</v>
+        <v>113</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" ht="60">
+      <c r="A50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G50" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="129.6">
-      <c r="B51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="120">
+      <c r="A51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="51">
-      <c r="B52" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>112</v>
+        <v>97</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="124.5">
+      <c r="A52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G52" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:7" ht="57.6">
-      <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="100.8">
-      <c r="A55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="103.2">
-      <c r="A56" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F56" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="100.8">
-      <c r="B57" t="s">
+      <c r="G52" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="120">
+      <c r="B53" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F53" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="42">
-      <c r="B58" t="s">
+      <c r="G53" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="57">
+      <c r="B54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C54" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F54" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="B60" t="s">
+      <c r="G54" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45">
+      <c r="B55" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C55" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="B62" t="s">
+      <c r="G55" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="B57" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C57" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="B63" t="s">
+      <c r="G57" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C58" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F58" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B59" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C59" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+      <c r="G59" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30">
+      <c r="A60" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B60" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C60" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="B66" t="s">
+    <row r="61" spans="1:7">
+      <c r="B61" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="B67" t="s">
+    <row r="62" spans="1:7" ht="30">
+      <c r="B62" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C62" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="B68" t="s">
+      <c r="G62" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30">
+      <c r="B63" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C63" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="B69" t="s">
+      <c r="G63" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="45">
+      <c r="B64" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C64" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="B70" t="s">
+      <c r="G64" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45">
+      <c r="B65" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C65" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="B72" t="s">
+      <c r="G65" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30">
+      <c r="B66" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C66" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="B73" t="s">
+      <c r="G66" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="60">
+      <c r="B67" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C67" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="B74" t="s">
+      <c r="G67" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="45">
+      <c r="B68" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C68" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+      <c r="G68" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B69" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C69" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="B77" t="s">
+      <c r="G69" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C71" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="B78" t="s">
+      <c r="G71" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="30">
+      <c r="B72" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C72" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="B79" t="s">
+      <c r="G72" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="B73" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C73" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="B80" t="s">
+      <c r="G73" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="30">
+      <c r="B74" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C74" s="2" t="s">
         <v>167</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F33" r:id="rId1" xr:uid="{35071A76-E82A-45DF-94C1-B3565D05B3A5}"/>
-    <hyperlink ref="F54" r:id="rId2" xr:uid="{C9B2AE1C-3EAD-40F7-938D-D5A949807441}"/>
-    <hyperlink ref="F55" r:id="rId3" xr:uid="{2B38F78D-8DA3-49B8-AD62-7E6F5FE37D4D}"/>
-    <hyperlink ref="F52" r:id="rId4" xr:uid="{65E66027-0BBA-4B7F-A2CE-D2C8CE3608DC}"/>
-    <hyperlink ref="F37" r:id="rId5" xr:uid="{AC9E3BB4-EA74-4CA9-BEDD-01FC4017C839}"/>
-    <hyperlink ref="F36" r:id="rId6" xr:uid="{AA3631C5-867E-49D0-A50B-49FA47F0CD13}"/>
-    <hyperlink ref="F48" r:id="rId7" xr:uid="{A4F46162-E510-4AC7-A468-B39513020E18}"/>
-    <hyperlink ref="F50" r:id="rId8" xr:uid="{F90C6926-B5D8-455C-8D0F-4E1136C4428B}"/>
-    <hyperlink ref="F51" r:id="rId9" xr:uid="{87142973-9B2A-451C-925A-74FE46AE2646}"/>
+    <hyperlink ref="F50" r:id="rId1" xr:uid="{C9B2AE1C-3EAD-40F7-938D-D5A949807441}"/>
+    <hyperlink ref="F51" r:id="rId2" xr:uid="{2B38F78D-8DA3-49B8-AD62-7E6F5FE37D4D}"/>
+    <hyperlink ref="F48" r:id="rId3" xr:uid="{65E66027-0BBA-4B7F-A2CE-D2C8CE3608DC}"/>
+    <hyperlink ref="F33" r:id="rId4" xr:uid="{AC9E3BB4-EA74-4CA9-BEDD-01FC4017C839}"/>
+    <hyperlink ref="F32" r:id="rId5" xr:uid="{AA3631C5-867E-49D0-A50B-49FA47F0CD13}"/>
+    <hyperlink ref="F44" r:id="rId6" xr:uid="{A4F46162-E510-4AC7-A468-B39513020E18}"/>
+    <hyperlink ref="F46" r:id="rId7" xr:uid="{F90C6926-B5D8-455C-8D0F-4E1136C4428B}"/>
+    <hyperlink ref="F47" r:id="rId8" xr:uid="{87142973-9B2A-451C-925A-74FE46AE2646}"/>
+    <hyperlink ref="F52" r:id="rId9" xr:uid="{60152650-AADB-4525-A844-D21A8BEF583E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -1876,56 +1947,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Team Document" ma:contentTypeID="0x010100A35317DCC28344A7B82488658A034A5C010069E498006C15F040AAF23C596505DB08" ma:contentTypeVersion="15" ma:contentTypeDescription=" " ma:contentTypeScope="" ma:versionID="daae089886e5dfcdf91620598e62335c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b267fd-bbe0-4fe3-86fd-466470c14b02" xmlns:ns3="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7" xmlns:ns5="46c07ff3-5521-42af-a653-3855c83cb6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c787740b624ceaa53a6f81b9ff22a49" ns2:_="" ns3:_="" ns5:_="">
     <xsd:import namespace="64b267fd-bbe0-4fe3-86fd-466470c14b02"/>
@@ -2238,7 +2259,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TNOC_ClusterId xmlns="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7">060.28387</TNOC_ClusterId>
@@ -2281,24 +2361,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC4FB55-D490-49ED-AEAA-963B2A830DFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC7E6127-10A1-40C5-9CAC-A18D42DD8A37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2318,7 +2381,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC4FB55-D490-49ED-AEAA-963B2A830DFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C697E9F-13EF-41CB-B4FF-229AEE100FCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4CA6ED-F389-43A6-8E29-AA59BC0B8044}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2334,12 +2413,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C697E9F-13EF-41CB-B4FF-229AEE100FCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>